<commit_message>
Add solution features for future development
</commit_message>
<xml_diff>
--- a/development/Lift_and_Cumulative_Lift_calculation.xlsx
+++ b/development/Lift_and_Cumulative_Lift_calculation.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BackUp - 151110\Side_Projects\Analytical_Solutions\Scorecard_Suite\development\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010D958F-E066-4D50-9696-9CB5C18ED45A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="18195" windowHeight="10035"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -19,15 +33,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Decile</t>
-  </si>
-  <si>
-    <t>Cumulative Responses</t>
-  </si>
-  <si>
-    <t>Number of Cases</t>
-  </si>
-  <si>
-    <t>Number of Responses</t>
   </si>
   <si>
     <t>Lift</t>
@@ -42,23 +47,32 @@
     <t>Cumulative % of Cases</t>
   </si>
   <si>
-    <t>Cumulative Cases</t>
-  </si>
-  <si>
     <t>Cumulative % of Events</t>
   </si>
   <si>
     <t>% of Events</t>
   </si>
+  <si>
+    <t># Cases</t>
+  </si>
+  <si>
+    <t># Responses</t>
+  </si>
+  <si>
+    <t>Cumulative # Responses</t>
+  </si>
+  <si>
+    <t>Cumulative # Cases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="181" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +87,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -82,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -90,17 +111,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -111,6 +154,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -159,7 +205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -192,9 +238,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,6 +290,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,498 +482,499 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" customWidth="1"/>
+    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>2500</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>2179</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <f>C2</f>
         <v>2179</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <f>C2/$C$12</f>
         <v>0.44706606483381206</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <f>D2/$C$12</f>
         <v>0.44706606483381206</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <f>B2/$B$12</f>
         <v>0.1</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <f>E2/G2</f>
         <v>4.4706606483381206</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <f>B2</f>
         <v>2500</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="5">
         <f>I2/$B$12</f>
         <v>0.1</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="6">
         <f>F2/J2</f>
         <v>4.4706606483381206</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2500</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>1753</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <f>C3+D2</f>
         <v>3932</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <f t="shared" ref="E3:E11" si="0">C3/$C$12</f>
         <v>0.35966352072219943</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <f t="shared" ref="F3:F11" si="1">D3/$C$12</f>
         <v>0.80672958555601149</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <f t="shared" ref="G3:G11" si="2">B3/$B$12</f>
         <v>0.1</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <f t="shared" ref="H3:H11" si="3">E3/G3</f>
         <v>3.5966352072219943</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <f>B3+I2</f>
         <v>5000</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="5">
         <f t="shared" ref="J3:J11" si="4">I3/$B$12</f>
         <v>0.2</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="6">
         <f t="shared" ref="K3:K11" si="5">F3/J3</f>
         <v>4.0336479277800574</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2500</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>396</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f t="shared" ref="D4:D11" si="6">C4+D3</f>
         <v>4328</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>8.1247435371358229E-2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <f t="shared" si="1"/>
         <v>0.88797702092736974</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="4">
         <f t="shared" si="3"/>
         <v>0.81247435371358223</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <f t="shared" ref="I4:I11" si="7">B4+I3</f>
         <v>7500</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="5">
         <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="6">
         <f t="shared" si="5"/>
         <v>2.9599234030912327</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>2500</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>111</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <f t="shared" si="6"/>
         <v>4439</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>2.2773902338941322E-2</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <f t="shared" si="1"/>
         <v>0.91075092326631102</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="4">
         <f t="shared" si="3"/>
         <v>0.22773902338941321</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <f t="shared" si="7"/>
         <v>10000</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="5">
         <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="6">
         <f t="shared" si="5"/>
         <v>2.2768773081657776</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>2500</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>110</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <f t="shared" si="6"/>
         <v>4549</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <f t="shared" si="0"/>
         <v>2.2568732047599509E-2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <f t="shared" si="1"/>
         <v>0.93331965531391059</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
         <f t="shared" si="3"/>
         <v>0.22568732047599507</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <f t="shared" si="7"/>
         <v>12500</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="5">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="6">
         <f t="shared" si="5"/>
         <v>1.8666393106278212</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>2500</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>85</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <f t="shared" si="6"/>
         <v>4634</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>1.7439474764054164E-2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <f t="shared" si="1"/>
         <v>0.95075913007796475</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="4">
         <f t="shared" si="3"/>
         <v>0.17439474764054164</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <f t="shared" si="7"/>
         <v>15000</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="5">
         <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="6">
         <f t="shared" si="5"/>
         <v>1.5845985501299413</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>2500</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>67</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <f t="shared" si="6"/>
         <v>4701</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>1.3746409519901519E-2</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <f t="shared" si="1"/>
         <v>0.96450553959786622</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <f t="shared" si="3"/>
         <v>0.13746409519901517</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <f t="shared" si="7"/>
         <v>17500</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="5">
         <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="6">
         <f t="shared" si="5"/>
         <v>1.3778650565683803</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>2500</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>69</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <f t="shared" si="6"/>
         <v>4770</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>1.4156750102585146E-2</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
         <f t="shared" si="1"/>
         <v>0.97866228970045133</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <f t="shared" si="3"/>
         <v>0.14156750102585144</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <f t="shared" si="7"/>
         <v>20000</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="5">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="6">
         <f t="shared" si="5"/>
         <v>1.2233278621255641</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>2500</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>49</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <f t="shared" si="6"/>
         <v>4819</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <f t="shared" si="0"/>
         <v>1.0053344275748872E-2</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="3">
         <f t="shared" si="1"/>
         <v>0.98871563397620021</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <f t="shared" si="3"/>
         <v>0.10053344275748871</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <f t="shared" si="7"/>
         <v>22500</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="5">
         <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="6">
         <f t="shared" si="5"/>
         <v>1.0985729266402224</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>2500</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>55</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <f t="shared" si="6"/>
         <v>4874</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <f t="shared" si="0"/>
         <v>1.1284366023799754E-2</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="3">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="4">
         <f t="shared" si="3"/>
         <v>0.11284366023799754</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <f t="shared" si="7"/>
         <v>25000</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" s="2">
         <f>SUM(B2:B11)</f>
         <v>25000</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <f>SUM(C2:C11)</f>
         <v>4874</v>
       </c>
@@ -905,24 +986,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>